<commit_message>
Simplified data update process
</commit_message>
<xml_diff>
--- a/DATA/SOURCE DATA/update_log.xlsx
+++ b/DATA/SOURCE DATA/update_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,15 +475,32 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Waitlist trend - statewide</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>14/01/2024</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>30/09/2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>Population (by State, Sex, Age to 65+)</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>14/01/2024</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>30/06/2023</t>
         </is>
@@ -771,29 +788,10 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="0f6d7760-f7d3-42f3-b5a6-16e4c400c838" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="208c7ed5-c894-4803-a7c7-831a8154db8b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Hyperlink xmlns="208c7ed5-c894-4803-a7c7-831a8154db8b">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Hyperlink>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AF7D678-1961-46CF-93E9-66F29B00B6FE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FB3C7AA-5185-4095-A945-72E0DFFCF1C2}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A52DD48B-F215-401E-9A7B-65453A1B39B4}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA4FFE-0BD6-41E7-9065-5328D698B530}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{783444C4-3022-4786-A4C8-C4AD689003D7}"/>
 </file>
</xml_diff>

<commit_message>
Sync 19 Jan reboot
</commit_message>
<xml_diff>
--- a/DATA/SOURCE DATA/update_log.xlsx
+++ b/DATA/SOURCE DATA/update_log.xlsx
@@ -463,7 +463,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>14/01/2024</t>
+          <t>16/01/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -789,9 +789,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFDAADA9-E7D0-4306-B594-6FA9E806A2FA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B0C3838-C25D-4409-9643-7E23E02EA05D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50543291-1D34-4086-A3C3-67ED3BA4AE99}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F97F890-9B8F-4212-97F3-7B36A1D8DD52}"/>
 </file>
</xml_diff>